<commit_message>
Ajout de plusieurs échantillons
Ajout échantillons et mise à jour du rapport de pic
</commit_message>
<xml_diff>
--- a/Rapport pic.xlsx
+++ b/Rapport pic.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAE635BE-D455-421F-8E29-DA5C8E57C476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maalo\OneDrive\Documents\GitHub\ProjetSTM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107C2787-4588-463D-AB83-E969F4430767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -15,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nom fichier</t>
   </si>
@@ -64,13 +58,28 @@
   </si>
   <si>
     <t>frelon6</t>
+  </si>
+  <si>
+    <t>frelon_bof</t>
+  </si>
+  <si>
+    <t>attaque_fre</t>
+  </si>
+  <si>
+    <t>frelon_nid</t>
+  </si>
+  <si>
+    <t>frelon_nid2</t>
+  </si>
+  <si>
+    <t>attaquev2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,10 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -431,18 +441,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G6"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -485,7 +495,7 @@
         <v>834.41200000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -505,7 +515,7 @@
         <v>715.97900000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -525,7 +535,7 @@
         <v>775.19500000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -543,6 +553,88 @@
       </c>
       <c r="F6">
         <v>780.779</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>161.499</v>
+      </c>
+      <c r="C7">
+        <v>253.01499999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>398.36399999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <v>479.11399999999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>559.86300000000006</v>
+      </c>
+      <c r="G7" s="3">
+        <v>640.61300000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>236.86500000000001</v>
+      </c>
+      <c r="C8">
+        <v>344.53100000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>468.34699999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>258.39800000000002</v>
+      </c>
+      <c r="C9">
+        <v>360.68099999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>473.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>258.39800000000002</v>
+      </c>
+      <c r="C10">
+        <v>387.59800000000001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>635.22900000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>231.482</v>
+      </c>
+      <c r="C11">
+        <v>360.68099999999998</v>
+      </c>
+      <c r="D11">
+        <v>457.58100000000002</v>
+      </c>
+      <c r="E11" s="3">
+        <v>602.92999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>